<commit_message>
Implement PDF file sorting and data extraction functionality
</commit_message>
<xml_diff>
--- a/python/yatirim_islemleri_extracted.xlsx
+++ b/python/yatirim_islemleri_extracted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\midas-vergi\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C1B1C8-9552-4D2C-87E8-964C39E37AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6D79BB-6C76-409D-9A4D-ECB4C14545E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="8940" yWindow="2805" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -780,7 +780,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -793,7 +795,10 @@
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add MongoDB integration and Excel processing for profit/loss calculation
</commit_message>
<xml_diff>
--- a/python/yatirim_islemleri_extracted.xlsx
+++ b/python/yatirim_islemleri_extracted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\midas-vergi\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6D79BB-6C76-409D-9A4D-ECB4C14545E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876C54AB-0D75-4F39-966D-CACB07657108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="8940" yWindow="2805" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2880" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -781,7 +781,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>